<commit_message>
Update statistic files for March 2024
</commit_message>
<xml_diff>
--- a/executive_board/2024_02_next_executive_board.xlsx
+++ b/executive_board/2024_02_next_executive_board.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2024\executive_board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\executive_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07542DF2-F741-4028-9D7C-8B870C49B983}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAB0ED9-ED7F-45A4-954B-1C6E80B141AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{76F7C32B-939B-4119-B411-60C078B28972}"/>
   </bookViews>
@@ -715,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83292FF-9AF5-4F08-A6AE-9A68B5623E13}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -756,457 +756,799 @@
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="B3" s="5">
+        <v>10542</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1870</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1934</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="7">
+        <v>6249</v>
+      </c>
+      <c r="C4" s="7">
+        <v>756</v>
+      </c>
+      <c r="D4" s="7">
+        <v>757</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="5">
+        <v>17692</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1847</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1896</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="7">
+        <v>294</v>
+      </c>
+      <c r="C6" s="7">
+        <v>185</v>
+      </c>
+      <c r="D6" s="7">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="5">
+        <v>12471</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2355</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1714</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="B8" s="7">
+        <v>1198</v>
+      </c>
+      <c r="C8" s="7">
+        <v>254</v>
+      </c>
+      <c r="D8" s="7">
+        <v>246</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="5">
+        <v>1276</v>
+      </c>
+      <c r="C9" s="5">
+        <v>324</v>
+      </c>
+      <c r="D9" s="5">
+        <v>190</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="7">
+        <v>558</v>
+      </c>
+      <c r="C10" s="7">
+        <v>107</v>
+      </c>
+      <c r="D10" s="7">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="5">
+        <v>166</v>
+      </c>
+      <c r="C11" s="5">
+        <v>90</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="9">
+        <v>321</v>
+      </c>
+      <c r="C13" s="9">
+        <v>66</v>
+      </c>
+      <c r="D13" s="9">
+        <v>123</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="11">
+        <v>743</v>
+      </c>
+      <c r="C14" s="11">
+        <v>352</v>
+      </c>
+      <c r="D14" s="11">
+        <v>370</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="9">
+        <v>1304</v>
+      </c>
+      <c r="C15" s="9">
+        <v>512</v>
+      </c>
+      <c r="D15" s="9">
+        <v>240</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="B16" s="11">
+        <v>808</v>
+      </c>
+      <c r="C16" s="11">
+        <v>507</v>
+      </c>
+      <c r="D16" s="11">
+        <v>109</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="5">
+        <v>607</v>
+      </c>
+      <c r="C17" s="5">
+        <v>229</v>
+      </c>
+      <c r="D17" s="5">
+        <v>94</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="B18" s="7">
+        <v>4178</v>
+      </c>
+      <c r="C18" s="7">
+        <v>672</v>
+      </c>
+      <c r="D18" s="7">
+        <v>885</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="B19" s="5">
+        <v>281</v>
+      </c>
+      <c r="C19" s="5">
+        <v>134</v>
+      </c>
+      <c r="D19" s="5">
+        <v>73</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="B20" s="7">
+        <v>4185</v>
+      </c>
+      <c r="C20" s="7">
+        <v>721</v>
+      </c>
+      <c r="D20" s="7">
+        <v>740</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="5">
+        <v>60</v>
+      </c>
+      <c r="C21" s="5">
+        <v>155</v>
+      </c>
+      <c r="D21" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="B22" s="7">
+        <v>3983</v>
+      </c>
+      <c r="C22" s="7">
+        <v>560</v>
+      </c>
+      <c r="D22" s="7">
+        <v>684</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="5">
+        <v>236</v>
+      </c>
+      <c r="C23" s="5">
+        <v>234</v>
+      </c>
+      <c r="D23" s="5">
+        <v>43</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="B24" s="7">
+        <v>5003</v>
+      </c>
+      <c r="C24" s="7">
+        <v>535</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1067</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="5">
+        <v>20394</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1789</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2764</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="B26" s="7">
+        <v>1580</v>
+      </c>
+      <c r="C26" s="7">
+        <v>456</v>
+      </c>
+      <c r="D26" s="7">
+        <v>226</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="7">
+        <v>1182</v>
+      </c>
+      <c r="C28" s="7">
+        <v>304</v>
+      </c>
+      <c r="D28" s="7">
+        <v>301</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="B29" s="5">
+        <v>391</v>
+      </c>
+      <c r="C29" s="5">
+        <v>158</v>
+      </c>
+      <c r="D29" s="5">
+        <v>105</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="B30" s="7">
+        <v>3190</v>
+      </c>
+      <c r="C30" s="7">
+        <v>651</v>
+      </c>
+      <c r="D30" s="7">
+        <v>843</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="5">
+        <v>122</v>
+      </c>
+      <c r="C31" s="5">
+        <v>20</v>
+      </c>
+      <c r="D31" s="5">
+        <v>85</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="B32" s="7">
+        <v>700</v>
+      </c>
+      <c r="C32" s="7">
+        <v>552</v>
+      </c>
+      <c r="D32" s="7">
+        <v>91</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="5">
+        <v>3276</v>
+      </c>
+      <c r="C33" s="5">
+        <v>899</v>
+      </c>
+      <c r="D33" s="5">
+        <v>771</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
+      <c r="B34" s="7">
+        <v>2339</v>
+      </c>
+      <c r="C34" s="7">
+        <v>831</v>
+      </c>
+      <c r="D34" s="7">
+        <v>484</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="B35" s="5">
+        <v>1235</v>
+      </c>
+      <c r="C35" s="5">
+        <v>162</v>
+      </c>
+      <c r="D35" s="5">
+        <v>231</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
+      <c r="B36" s="7">
+        <v>14022</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1736</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1378</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="B37" s="5">
+        <v>2071</v>
+      </c>
+      <c r="C37" s="5">
+        <v>782</v>
+      </c>
+      <c r="D37" s="5">
+        <v>327</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="B38" s="7">
+        <v>6478</v>
+      </c>
+      <c r="C38" s="7">
+        <v>456</v>
+      </c>
+      <c r="D38" s="7">
+        <v>675</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="B39" s="5">
+        <v>165</v>
+      </c>
+      <c r="C39" s="5">
+        <v>300</v>
+      </c>
+      <c r="D39" s="5">
+        <v>40</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
+      <c r="B40" s="7">
+        <v>299</v>
+      </c>
+      <c r="C40" s="7">
+        <v>135</v>
+      </c>
+      <c r="D40" s="7">
+        <v>100</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
+      <c r="B41" s="13">
+        <v>833</v>
+      </c>
+      <c r="C41" s="13">
+        <v>246</v>
+      </c>
+      <c r="D41" s="13">
+        <v>55</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
+      <c r="B42" s="15">
+        <v>3756</v>
+      </c>
+      <c r="C42" s="15">
+        <v>147</v>
+      </c>
+      <c r="D42" s="15">
+        <v>179</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
+      <c r="B43" s="13">
+        <v>88</v>
+      </c>
+      <c r="C43" s="13">
+        <v>59</v>
+      </c>
+      <c r="D43" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
+      <c r="B44" s="15">
+        <v>278</v>
+      </c>
+      <c r="C44" s="15">
+        <v>58</v>
+      </c>
+      <c r="D44" s="15">
+        <v>27</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
+      <c r="B45" s="13">
+        <v>0</v>
+      </c>
+      <c r="C45" s="13">
+        <v>0</v>
+      </c>
+      <c r="D45" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
+      <c r="B46" s="7">
+        <v>810</v>
+      </c>
+      <c r="C46" s="7">
+        <v>281</v>
+      </c>
+      <c r="D46" s="7">
+        <v>99</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="B47" s="5">
+        <v>3539</v>
+      </c>
+      <c r="C47" s="5">
+        <v>980</v>
+      </c>
+      <c r="D47" s="5">
+        <v>729</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
+      <c r="B48" s="7">
+        <v>7780</v>
+      </c>
+      <c r="C48" s="7">
+        <v>1013</v>
+      </c>
+      <c r="D48" s="7">
+        <v>1416</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="B49" s="5">
+        <v>3413</v>
+      </c>
+      <c r="C49" s="5">
+        <v>1081</v>
+      </c>
+      <c r="D49" s="5">
+        <v>439</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
+      <c r="B50" s="7">
+        <v>2819</v>
+      </c>
+      <c r="C50" s="7">
+        <v>361</v>
+      </c>
+      <c r="D50" s="7">
+        <v>656</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="B51" s="5">
+        <v>8272</v>
+      </c>
+      <c r="C51" s="5">
+        <v>777</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1417</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
+      <c r="B52" s="7">
+        <v>1051</v>
+      </c>
+      <c r="C52" s="7">
+        <v>276</v>
+      </c>
+      <c r="D52" s="7">
+        <v>315</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="B53" s="5">
+        <v>2909</v>
+      </c>
+      <c r="C53" s="5">
+        <v>563</v>
+      </c>
+      <c r="D53" s="5">
+        <v>511</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
+      <c r="B54" s="7">
+        <v>545</v>
+      </c>
+      <c r="C54" s="7">
+        <v>355</v>
+      </c>
+      <c r="D54" s="7">
+        <v>211</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="B55" s="5">
+        <v>635</v>
+      </c>
+      <c r="C55" s="5">
+        <v>391</v>
+      </c>
+      <c r="D55" s="5">
+        <v>31</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
+      <c r="B56" s="7">
+        <v>1414</v>
+      </c>
+      <c r="C56" s="7">
+        <v>346</v>
+      </c>
+      <c r="D56" s="7">
+        <v>438</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
+      <c r="B57" s="17">
+        <v>3176</v>
+      </c>
+      <c r="C57" s="17">
+        <v>1437</v>
+      </c>
+      <c r="D57" s="17">
+        <v>842</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
+      <c r="B58" s="19">
+        <v>4955</v>
+      </c>
+      <c r="C58" s="19">
+        <v>510</v>
+      </c>
+      <c r="D58" s="19">
+        <v>264</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="B59" s="21">
+        <v>167741</v>
+      </c>
+      <c r="C59" s="21">
+        <v>28630</v>
+      </c>
+      <c r="D59" s="21">
+        <v>26212</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D2" xr:uid="{2BAA0360-28EA-43C5-949A-024CCEDC735A}"/>

</xml_diff>